<commit_message>
Some improvements to GND/AGND track impedance around FB1 and some clearance changes.
</commit_message>
<xml_diff>
--- a/bom-nz-element14.xlsx
+++ b/bom-nz-element14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11760" yWindow="4140" windowWidth="21720" windowHeight="12260" tabRatio="500"/>
+    <workbookView xWindow="1020" yWindow="480" windowWidth="21720" windowHeight="12260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="bom.csv" sheetId="1" r:id="rId1"/>
@@ -344,10 +344,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -427,12 +425,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -446,7 +444,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -780,7 +778,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1678,7 +1676,6 @@
     </row>
     <row r="30" spans="1:11" ht="14" thickTop="1"/>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G7" r:id="rId1" display="http://nz.element14.com/avx/dp/1658140"/>
@@ -1705,7 +1702,6 @@
     <hyperlink ref="G28" r:id="rId22" display="http://nz.element14.com/txc/dp/1892154"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>